<commit_message>
lat lng API implemented
</commit_message>
<xml_diff>
--- a/effiko.xlsx
+++ b/effiko.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\effiko-api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\effiko-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCCFECC-D394-40C7-98D1-20B78DBD9299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC351C62-6998-4482-960E-613B33F5E642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9B9954AE-27A8-4982-954F-66D15F794264}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B9954AE-27A8-4982-954F-66D15F794264}"/>
   </bookViews>
   <sheets>
     <sheet name="Figma Queries" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>User</t>
   </si>
@@ -131,9 +131,6 @@
     <t>ContactUs</t>
   </si>
   <si>
-    <t>message</t>
-  </si>
-  <si>
     <t>Locations</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>linkedIn-data</t>
   </si>
   <si>
-    <t>linkedin-email</t>
-  </si>
-  <si>
     <t>cv (pdf)</t>
   </si>
   <si>
@@ -206,9 +200,6 @@
     <t>Interviews</t>
   </si>
   <si>
-    <t>link (youtube)</t>
-  </si>
-  <si>
     <t>User Register &amp; Login Pages ?</t>
   </si>
   <si>
@@ -219,6 +210,18 @@
   </si>
   <si>
     <t>linkedin_url</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>linkedin_email</t>
+  </si>
+  <si>
+    <t>book (pdf)</t>
   </si>
 </sst>
 </file>
@@ -681,9 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC103FC8-C95E-4CF1-9B65-D60B0A1C9F20}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -693,10 +694,11 @@
     <col min="4" max="4" width="21" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="16" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -710,7 +712,7 @@
         <v>27</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>23</v>
@@ -718,20 +720,20 @@
       <c r="F1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>55</v>
+      <c r="H1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -745,7 +747,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>24</v>
@@ -753,19 +755,19 @@
       <c r="F2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="G2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -777,7 +779,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>28</v>
@@ -788,16 +790,16 @@
       <c r="F3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="I3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>28</v>
       </c>
     </row>
@@ -818,17 +820,17 @@
       <c r="F4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="G4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="K4" t="s">
-        <v>56</v>
+      <c r="K4" s="10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -836,18 +838,21 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -857,44 +862,44 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -904,37 +909,37 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>